<commit_message>
trying to use caret
</commit_message>
<xml_diff>
--- a/R-course/dataset/Titanic Passengers.xlsx
+++ b/R-course/dataset/Titanic Passengers.xlsx
@@ -6030,7 +6030,7 @@
   <dimension ref="A1:L1310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51989,6 +51989,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FACE5D818E5F50479853446EE507747E" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5fbcd5a948c1c01ccdfc4c5d3323d2ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d3de4b96-056f-41d8-923d-53addee4e8b2" xmlns:ns4="4b297ba6-3c75-43f4-b046-b7dedaa9211e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="189605b7f6f153be8090590aee5976aa" ns3:_="" ns4:_="">
     <xsd:import namespace="d3de4b96-056f-41d8-923d-53addee4e8b2"/>
@@ -52209,15 +52218,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -52227,6 +52227,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6BEE55-632D-4715-898D-32324E8D77E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98649D0F-BA04-4B89-ABD7-11600220E0FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -52245,25 +52253,17 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6BEE55-632D-4715-898D-32324E8D77E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAA019B-4695-45A8-9703-04BBF7D8F83A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="d3de4b96-056f-41d8-923d-53addee4e8b2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="4b297ba6-3c75-43f4-b046-b7dedaa9211e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d3de4b96-056f-41d8-923d-53addee4e8b2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>

</xml_diff>